<commit_message>
add app-ui folder with homepage code
</commit_message>
<xml_diff>
--- a/Plan-Docs/Project - Story-Shpere Report.xlsx
+++ b/Plan-Docs/Project - Story-Shpere Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatarohithkola/Downloads/CC/Go/Story-Sphere/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatarohithkola/Downloads/CC/Go/Story-Sphere/Plan-Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E812A4B-391F-5545-88C9-A0C98F72196C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29878D1A-86A7-774A-A675-FDB9B940F181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Project Objective</t>
   </si>
@@ -166,6 +166,12 @@
   <si>
     <t>Explore the database options</t>
   </si>
+  <si>
+    <t>Not Done</t>
+  </si>
+  <si>
+    <t>Design Login Page and Write Story page</t>
+  </si>
 </sst>
 </file>
 
@@ -226,15 +232,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -294,11 +312,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -330,21 +363,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -819,11 +866,11 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -28693,10 +28740,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:Y11"/>
+  <dimension ref="A2:Y13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -28709,11 +28756,11 @@
   <sheetData>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10"/>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -28738,16 +28785,16 @@
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="16" t="s">
         <v>31</v>
       </c>
       <c r="F3" s="10"/>
@@ -28773,16 +28820,16 @@
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
-      <c r="B4" s="12">
+      <c r="B4" s="17">
         <v>45610</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="21" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="10"/>
@@ -28808,16 +28855,16 @@
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
-      <c r="B5" s="12">
+      <c r="B5" s="17">
         <v>45610</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="21" t="s">
         <v>34</v>
       </c>
       <c r="F5" s="10"/>
@@ -28843,16 +28890,16 @@
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
-      <c r="B6" s="12">
+      <c r="B6" s="17">
         <v>45610</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="21" t="s">
         <v>34</v>
       </c>
       <c r="F6" s="10"/>
@@ -28878,16 +28925,16 @@
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
-      <c r="B7" s="12">
+      <c r="B7" s="17">
         <v>45611</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="18">
         <v>1.5</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="21" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="10"/>
@@ -28913,16 +28960,16 @@
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
-      <c r="B8" s="12">
+      <c r="B8" s="17">
         <v>45611</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="18">
         <v>1.5</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="21" t="s">
         <v>34</v>
       </c>
       <c r="F8" s="10"/>
@@ -28948,16 +28995,16 @@
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
-      <c r="B9" s="12">
+      <c r="B9" s="17">
         <v>45611</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="18">
         <v>1</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="22" t="s">
         <v>34</v>
       </c>
       <c r="F9" s="10"/>
@@ -28983,16 +29030,18 @@
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
-      <c r="B10" s="12">
+      <c r="B10" s="17">
         <v>45612</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="18">
         <v>4</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="22" t="s">
+        <v>34</v>
+      </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
@@ -29016,16 +29065,18 @@
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10"/>
-      <c r="B11" s="12">
+      <c r="B11" s="17">
         <v>45612</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="18">
         <v>1</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="23" t="s">
+        <v>42</v>
+      </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -29047,6 +29098,30 @@
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
     </row>
+    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="17">
+        <v>45613</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="18">
+        <v>1</v>
+      </c>
+      <c r="E12" s="19"/>
+    </row>
+    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="17">
+        <v>45613</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="20">
+        <v>4</v>
+      </c>
+      <c r="E13" s="19"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
modify Login Main Write pages
</commit_message>
<xml_diff>
--- a/Plan-Docs/Project - Story-Shpere Report.xlsx
+++ b/Plan-Docs/Project - Story-Shpere Report.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatarohithkola/Downloads/CC/Go/Story-Sphere/Plan-Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29878D1A-86A7-774A-A675-FDB9B940F181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B2EA65-4267-534C-8D77-DB90B6BE10BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
-    <sheet name="Progress" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Project Objective</t>
   </si>
@@ -124,63 +123,12 @@
   <si>
     <t>Integrate frontend with backend APIs</t>
   </si>
-  <si>
-    <t>Daily Task Progress Report</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Hours</t>
-  </si>
-  <si>
-    <t>Worklog</t>
-  </si>
-  <si>
-    <t>Define Project Objective</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Define roles and their features</t>
-  </si>
-  <si>
-    <t>Define requiremnets and estimation</t>
-  </si>
-  <si>
-    <t>Researched 3 similar platforms for inspiration</t>
-  </si>
-  <si>
-    <t>Created UI prototype in Figma</t>
-  </si>
-  <si>
-    <t>Explore the Frontend tech to be used</t>
-  </si>
-  <si>
-    <t>Design Homepage</t>
-  </si>
-  <si>
-    <t>Explore the database options</t>
-  </si>
-  <si>
-    <t>Not Done</t>
-  </si>
-  <si>
-    <t>Design Login Page and Write Story page</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mmm\ d"/>
-  </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -217,42 +165,16 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -312,26 +234,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -360,40 +267,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,7 +492,7 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -866,11 +744,11 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -28733,399 +28611,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A2:Y13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" customWidth="1"/>
-    <col min="3" max="3" width="35.5" customWidth="1"/>
-    <col min="5" max="5" width="35.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="10"/>
-      <c r="B2" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-    </row>
-    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="10"/>
-      <c r="B3" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-    </row>
-    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="10"/>
-      <c r="B4" s="17">
-        <v>45610</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-    </row>
-    <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="10"/>
-      <c r="B5" s="17">
-        <v>45610</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10"/>
-    </row>
-    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="10"/>
-      <c r="B6" s="17">
-        <v>45610</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-    </row>
-    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="10"/>
-      <c r="B7" s="17">
-        <v>45611</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="18">
-        <v>1.5</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="10"/>
-    </row>
-    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="10"/>
-      <c r="B8" s="17">
-        <v>45611</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="18">
-        <v>1.5</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
-    </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="10"/>
-      <c r="B9" s="17">
-        <v>45611</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="18">
-        <v>1</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
-    </row>
-    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="10"/>
-      <c r="B10" s="17">
-        <v>45612</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="18">
-        <v>4</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-    </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="10"/>
-      <c r="B11" s="17">
-        <v>45612</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="18">
-        <v>1</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
-      <c r="X11" s="10"/>
-      <c r="Y11" s="10"/>
-    </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="17">
-        <v>45613</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="18">
-        <v>1</v>
-      </c>
-      <c r="E12" s="19"/>
-    </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="17">
-        <v>45613</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="20">
-        <v>4</v>
-      </c>
-      <c r="E13" s="19"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:E2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>